<commit_message>
Update result calculation sheet.xlsx
</commit_message>
<xml_diff>
--- a/result calculation sheet.xlsx
+++ b/result calculation sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ferdous\Documents\GitHub\result_calculation_excel_sheet\result_calculation_excel_sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ferdous\Documents\GitHub\result_calculation_excel_sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DCD370-FC01-4328-B337-50FBD1526767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF7D3A7-8734-467C-9211-155FB7CC31BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86089DA0-2BA1-4133-B16D-0F30CFEF8E2B}"/>
   </bookViews>
@@ -830,8 +830,8 @@
   </sheetPr>
   <dimension ref="A1:AH63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.21875" defaultRowHeight="15" x14ac:dyDescent="0.35"/>

</xml_diff>